<commit_message>
Hjemme passive - complete run
</commit_message>
<xml_diff>
--- a/data_output/prism_passive/all_passive_ROM common (all subjects).xlsx
+++ b/data_output/prism_passive/all_passive_ROM common (all subjects).xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\MATLAB\tend_stiff_2\data_output\prism_passive\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11364" windowHeight="6744"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -342,7 +337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -356,7 +351,7 @@
       <selection activeCell="B1" sqref="B1:AY3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Hjemme passive tweaks lichtwark deleted values
</commit_message>
<xml_diff>
--- a/data_output/prism_passive/all_passive_ROM common (all subjects).xlsx
+++ b/data_output/prism_passive/all_passive_ROM common (all subjects).xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\MATLAB\tend_stiff_2\data_output\prism_passive\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -342,7 +337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -353,26 +348,26 @@
   <dimension ref="A1:AY3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AY3"/>
+      <selection activeCell="B1" sqref="B1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F1">
         <v>5</v>

</xml_diff>

<commit_message>
Hjemme passive updated meanEMG legmaxROM
</commit_message>
<xml_diff>
--- a/data_output/prism_passive/all_passive_ROM common (all subjects).xlsx
+++ b/data_output/prism_passive/all_passive_ROM common (all subjects).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\MATLAB\tend_stiff_2\data_output\prism_passive\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -342,7 +337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -353,26 +348,26 @@
   <dimension ref="A1:AY3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AY3"/>
+      <selection activeCell="B1" sqref="B1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F1">
         <v>5</v>

</xml_diff>